<commit_message>
execution and scoring of lake model works
</commit_message>
<xml_diff>
--- a/Data/calibration_data/final_proc_genes_metaWRAP.xlsx
+++ b/Data/calibration_data/final_proc_genes_metaWRAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/login/Documents/MysticLakeBins/MWMW/Data/calibration_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68C87A5-7795-FB49-A7D3-4EACFD901BFF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E78F69D-DA57-4640-85F4-AF49C8C5D066}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="20" windowWidth="28560" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,10 +118,10 @@
     <t>Methanogenesis</t>
   </si>
   <si>
-    <t>C1 oxidation (Sum)</t>
-  </si>
-  <si>
     <t>Iron Reduction</t>
+  </si>
+  <si>
+    <t>C1 Oxidation (Sum)</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -944,7 +944,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>5.0945023449591599E-2</v>
@@ -994,7 +994,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>3.09354637360999E-2</v>
@@ -1044,7 +1044,7 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11">
         <v>4.4719835910273099E-2</v>
@@ -1094,7 +1094,7 @@
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>2.6018242263419498E-2</v>
@@ -1144,7 +1144,7 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>3.4738407842320899E-2</v>

</xml_diff>